<commit_message>
Added missing contact sap id
</commit_message>
<xml_diff>
--- a/src/test/data/contracts-import-false-data.xlsx
+++ b/src/test/data/contracts-import-false-data.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">Sopimuksen SAP-tunnus</t>
+  </si>
   <si>
     <t xml:space="preserve">Viljelijän SAP-tunnus</t>
   </si>
@@ -43,6 +46,12 @@
     <t xml:space="preserve">SAP-kommentti</t>
   </si>
   <si>
+    <t xml:space="preserve">fakeSapContractId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fakeSapContactId</t>
+  </si>
+  <si>
     <t xml:space="preserve">304100/Mansikka</t>
   </si>
   <si>
@@ -52,7 +61,7 @@
     <t xml:space="preserve">Kyllä</t>
   </si>
   <si>
-    <t xml:space="preserve">01</t>
+    <t xml:space="preserve">fakeDPSapId</t>
   </si>
 </sst>
 </file>
@@ -63,7 +72,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -84,6 +93,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,12 +142,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -154,22 +172,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -185,11 +204,11 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="n">
         <v>100</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>4</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>5</v>
@@ -197,28 +216,34 @@
       <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>301274</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>